<commit_message>
EPSCOR Auto stash before merge of "main" and "origin/main"
</commit_message>
<xml_diff>
--- a/221116_TDP.xlsx
+++ b/221116_TDP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://univalaska-my.sharepoint.com/personal/jadams125_alaska_edu/Documents/GitHub/UAF-Metabolism/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_2897\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_0F5FE257568FFC52273DFB9690FE36C1F31AB8AB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E73D5F9-D396-40BE-B9C7-DD5A919F0916}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_0F5FE257568FFC52273DFB9690FE36C1F31AB8AB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="12930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -408,18 +408,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -434,11 +428,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="22" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -725,23 +717,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93:J94"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>103</v>
       </c>
@@ -767,7 +759,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -787,7 +779,7 @@
         <v>44881.674780092595</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -807,7 +799,7 @@
         <v>44881.674988425926</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -827,7 +819,7 @@
         <v>44881.675613425927</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -847,7 +839,7 @@
         <v>44881.675821759258</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -867,7 +859,7 @@
         <v>44881.676446759258</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -887,7 +879,7 @@
         <v>44881.676655092589</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -907,7 +899,7 @@
         <v>44881.67728009259</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -927,7 +919,7 @@
         <v>44881.677488425928</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -947,7 +939,7 @@
         <v>44881.678113425929</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -967,7 +959,7 @@
         <v>44881.67832175926</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -987,7 +979,7 @@
         <v>44881.678946759261</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1007,7 +999,7 @@
         <v>44881.679155092592</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1033,7 +1025,7 @@
         <v>44881.679780092592</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1059,7 +1051,7 @@
         <v>44881.679988425924</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1085,7 +1077,7 @@
         <v>44881.680625000001</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1105,7 +1097,7 @@
         <v>44881.680821759262</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1125,7 +1117,7 @@
         <v>44881.681458333333</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1145,7 +1137,7 @@
         <v>44881.681655092594</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1165,7 +1157,7 @@
         <v>44881.682291666664</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1191,7 +1183,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1217,7 +1209,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>346</v>
       </c>
@@ -1243,7 +1235,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -1269,7 +1261,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>103</v>
       </c>
@@ -1295,7 +1287,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1321,7 +1313,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -1347,7 +1339,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -1373,7 +1365,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -1399,7 +1391,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>25</v>
       </c>
@@ -1425,7 +1417,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -1451,7 +1443,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -1477,7 +1469,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -1503,7 +1495,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -1529,7 +1521,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -1555,7 +1547,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -1581,7 +1573,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>32</v>
       </c>
@@ -1607,7 +1599,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>33</v>
       </c>
@@ -1633,63 +1625,59 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A39" s="2" t="s">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39">
         <v>12</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39">
         <v>0.52700000000000002</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39">
         <v>9.9000000000000008E-3</v>
       </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2">
-        <v>0</v>
-      </c>
-      <c r="H39" s="3">
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39" s="1">
         <v>44881.69</v>
       </c>
-      <c r="I39" s="2" t="s">
+      <c r="I39" t="s">
         <v>111</v>
       </c>
-      <c r="J39" s="2">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A40" s="2" t="s">
+      <c r="J39">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40">
         <v>12</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40">
         <v>0.45300000000000001</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40">
         <v>8.6E-3</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2">
+      <c r="G40">
         <v>14.99</v>
       </c>
-      <c r="H40" s="3">
+      <c r="H40" s="1">
         <v>44881.690625000003</v>
       </c>
-      <c r="I40" s="2" t="s">
+      <c r="I40" t="s">
         <v>111</v>
       </c>
-      <c r="J40" s="2">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J40">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -1718,7 +1706,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -1750,7 +1738,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>11</v>
       </c>
@@ -1779,7 +1767,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>36</v>
       </c>
@@ -1805,7 +1793,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>37</v>
       </c>
@@ -1831,7 +1819,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>149</v>
       </c>
@@ -1857,7 +1845,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>38</v>
       </c>
@@ -1883,7 +1871,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>39</v>
       </c>
@@ -1909,7 +1897,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>40</v>
       </c>
@@ -1935,7 +1923,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>41</v>
       </c>
@@ -1961,7 +1949,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>42</v>
       </c>
@@ -1987,7 +1975,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>43</v>
       </c>
@@ -2007,7 +1995,7 @@
         <v>44881.695625</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>44</v>
       </c>
@@ -2030,7 +2018,7 @@
         <v>44881.695833333331</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>46</v>
       </c>
@@ -2056,7 +2044,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>47</v>
       </c>
@@ -2082,7 +2070,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>48</v>
       </c>
@@ -2108,7 +2096,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>49</v>
       </c>
@@ -2134,7 +2122,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>912</v>
       </c>
@@ -2160,7 +2148,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>50</v>
       </c>
@@ -2186,7 +2174,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>9458</v>
       </c>
@@ -2212,7 +2200,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>51</v>
       </c>
@@ -2238,7 +2226,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>52</v>
       </c>
@@ -2264,7 +2252,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>53</v>
       </c>
@@ -2290,7 +2278,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>54</v>
       </c>
@@ -2316,7 +2304,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>55</v>
       </c>
@@ -2342,7 +2330,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>56</v>
       </c>
@@ -2368,7 +2356,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>57</v>
       </c>
@@ -2394,7 +2382,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>4</v>
       </c>
@@ -2426,7 +2414,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>8</v>
       </c>
@@ -2458,7 +2446,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>11</v>
       </c>
@@ -2490,7 +2478,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>58</v>
       </c>
@@ -2516,7 +2504,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>59</v>
       </c>
@@ -2542,7 +2530,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>60</v>
       </c>
@@ -2568,7 +2556,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>61</v>
       </c>
@@ -2594,7 +2582,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>62</v>
       </c>
@@ -2620,7 +2608,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>63</v>
       </c>
@@ -2646,7 +2634,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>64</v>
       </c>
@@ -2672,7 +2660,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>65</v>
       </c>
@@ -2698,7 +2686,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>66</v>
       </c>
@@ -2724,7 +2712,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>67</v>
       </c>
@@ -2750,7 +2738,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>68</v>
       </c>
@@ -2776,7 +2764,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>69</v>
       </c>
@@ -2802,7 +2790,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>70</v>
       </c>
@@ -2828,7 +2816,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>71</v>
       </c>
@@ -2854,7 +2842,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>72</v>
       </c>
@@ -2880,7 +2868,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>73</v>
       </c>
@@ -2906,7 +2894,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>74</v>
       </c>
@@ -2932,7 +2920,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>75</v>
       </c>
@@ -2958,7 +2946,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>76</v>
       </c>
@@ -2984,7 +2972,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>77</v>
       </c>
@@ -3010,7 +2998,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>78</v>
       </c>
@@ -3036,7 +3024,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>79</v>
       </c>
@@ -3062,63 +3050,59 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A93" s="2" t="s">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>80</v>
       </c>
-      <c r="B93" s="2">
+      <c r="B93">
         <v>36</v>
       </c>
-      <c r="C93" s="2">
+      <c r="C93">
         <v>0.126</v>
       </c>
-      <c r="D93" s="2">
+      <c r="D93">
         <v>2.8E-3</v>
       </c>
-      <c r="E93" s="2"/>
-      <c r="F93" s="2"/>
-      <c r="G93" s="2">
-        <v>0</v>
-      </c>
-      <c r="H93" s="3">
+      <c r="G93">
+        <v>0</v>
+      </c>
+      <c r="H93" s="1">
         <v>44881.712511574071</v>
       </c>
-      <c r="I93" s="2" t="s">
+      <c r="I93" t="s">
         <v>113</v>
       </c>
-      <c r="J93" s="2">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A94" s="2" t="s">
+      <c r="J93">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>81</v>
       </c>
-      <c r="B94" s="2">
+      <c r="B94">
         <v>36</v>
       </c>
-      <c r="C94" s="2">
+      <c r="C94">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="D94" s="2">
+      <c r="D94">
         <v>1.4E-3</v>
       </c>
-      <c r="E94" s="2"/>
-      <c r="F94" s="2"/>
-      <c r="G94" s="2">
+      <c r="G94">
         <v>91.95</v>
       </c>
-      <c r="H94" s="3">
+      <c r="H94" s="1">
         <v>44881.713136574072</v>
       </c>
-      <c r="I94" s="2" t="s">
+      <c r="I94" t="s">
         <v>113</v>
       </c>
-      <c r="J94" s="2">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J94">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>4</v>
       </c>
@@ -3147,7 +3131,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>8</v>
       </c>
@@ -3179,7 +3163,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>11</v>
       </c>
@@ -3211,119 +3195,111 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A98" s="2" t="s">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>82</v>
       </c>
-      <c r="B98" s="2">
+      <c r="B98">
         <v>37</v>
       </c>
-      <c r="C98" s="2">
+      <c r="C98">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="D98" s="2">
+      <c r="D98">
         <v>2.0999999999999999E-3</v>
       </c>
-      <c r="E98" s="2"/>
-      <c r="F98" s="2"/>
-      <c r="G98" s="2">
-        <v>0</v>
-      </c>
-      <c r="H98" s="3">
+      <c r="G98">
+        <v>0</v>
+      </c>
+      <c r="H98" s="1">
         <v>44881.714803240742</v>
       </c>
-      <c r="I98" s="2" t="s">
+      <c r="I98" t="s">
         <v>113</v>
       </c>
-      <c r="J98" s="2">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A99" s="2" t="s">
+      <c r="J98">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>83</v>
       </c>
-      <c r="B99" s="2">
+      <c r="B99">
         <v>37</v>
       </c>
-      <c r="C99" s="2">
+      <c r="C99">
         <v>0.126</v>
       </c>
-      <c r="D99" s="2">
+      <c r="D99">
         <v>2.8E-3</v>
       </c>
-      <c r="E99" s="2"/>
-      <c r="F99" s="2"/>
-      <c r="G99" s="2">
+      <c r="G99">
         <v>-37.380000000000003</v>
       </c>
-      <c r="H99" s="3">
+      <c r="H99" s="1">
         <v>44881.71502314815</v>
       </c>
-      <c r="I99" s="2" t="s">
+      <c r="I99" t="s">
         <v>113</v>
       </c>
-      <c r="J99" s="2">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A100" s="2">
+      <c r="J99">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100">
         <v>10755</v>
       </c>
-      <c r="B100" s="2">
+      <c r="B100">
         <v>38</v>
       </c>
-      <c r="C100" s="2">
+      <c r="C100">
         <v>0.10299999999999999</v>
       </c>
-      <c r="D100" s="2">
+      <c r="D100">
         <v>2.3999999999999998E-3</v>
       </c>
-      <c r="E100" s="2"/>
-      <c r="F100" s="2"/>
-      <c r="G100" s="2">
-        <v>0</v>
-      </c>
-      <c r="H100" s="3">
+      <c r="G100">
+        <v>0</v>
+      </c>
+      <c r="H100" s="1">
         <v>44881.715648148151</v>
       </c>
-      <c r="I100" s="2" t="s">
+      <c r="I100" t="s">
         <v>113</v>
       </c>
-      <c r="J100" s="2">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A101" s="2" t="s">
+      <c r="J100">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>84</v>
       </c>
-      <c r="B101" s="2">
+      <c r="B101">
         <v>38</v>
       </c>
-      <c r="C101" s="2">
+      <c r="C101">
         <v>0.188</v>
       </c>
-      <c r="D101" s="2">
+      <c r="D101">
         <v>3.8999999999999998E-3</v>
       </c>
-      <c r="E101" s="2"/>
-      <c r="F101" s="2"/>
-      <c r="G101" s="2">
+      <c r="G101">
         <v>-58.31</v>
       </c>
-      <c r="H101" s="3">
+      <c r="H101" s="1">
         <v>44881.715856481482</v>
       </c>
-      <c r="I101" s="2" t="s">
+      <c r="I101" t="s">
         <v>113</v>
       </c>
-      <c r="J101" s="2">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J101">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>85</v>
       </c>
@@ -3349,7 +3325,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>86</v>
       </c>
@@ -3375,7 +3351,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>9466</v>
       </c>
@@ -3401,7 +3377,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>87</v>
       </c>
@@ -3427,63 +3403,59 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A106" s="2" t="s">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>88</v>
       </c>
-      <c r="B106" s="2">
+      <c r="B106">
         <v>41</v>
       </c>
-      <c r="C106" s="2">
+      <c r="C106">
         <v>0.126</v>
       </c>
-      <c r="D106" s="2">
+      <c r="D106">
         <v>2.8E-3</v>
       </c>
-      <c r="E106" s="2"/>
-      <c r="F106" s="2"/>
-      <c r="G106" s="2">
-        <v>0</v>
-      </c>
-      <c r="H106" s="3">
+      <c r="G106">
+        <v>0</v>
+      </c>
+      <c r="H106" s="1">
         <v>44881.718148148146</v>
       </c>
-      <c r="I106" s="2" t="s">
+      <c r="I106" t="s">
         <v>113</v>
       </c>
-      <c r="J106" s="2">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A107" s="2" t="s">
+      <c r="J106">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>89</v>
       </c>
-      <c r="B107" s="2">
+      <c r="B107">
         <v>41</v>
       </c>
-      <c r="C107" s="2">
+      <c r="C107">
         <v>0.182</v>
       </c>
-      <c r="D107" s="2">
+      <c r="D107">
         <v>3.8E-3</v>
       </c>
-      <c r="E107" s="2"/>
-      <c r="F107" s="2"/>
-      <c r="G107" s="2">
+      <c r="G107">
         <v>-36.729999999999997</v>
       </c>
-      <c r="H107" s="3">
+      <c r="H107" s="1">
         <v>44881.718356481484</v>
       </c>
-      <c r="I107" s="2" t="s">
+      <c r="I107" t="s">
         <v>113</v>
       </c>
-      <c r="J107" s="2">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J107">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>7552</v>
       </c>
@@ -3509,7 +3481,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>90</v>
       </c>
@@ -3535,7 +3507,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>91</v>
       </c>
@@ -3561,7 +3533,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>92</v>
       </c>
@@ -3587,7 +3559,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>93</v>
       </c>
@@ -3613,7 +3585,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>94</v>
       </c>
@@ -3639,7 +3611,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>95</v>
       </c>
@@ -3665,7 +3637,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>96</v>
       </c>
@@ -3691,63 +3663,59 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A116" s="2" t="s">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>97</v>
       </c>
-      <c r="B116" s="2">
+      <c r="B116">
         <v>46</v>
       </c>
-      <c r="C116" s="2">
+      <c r="C116">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="D116" s="2">
+      <c r="D116">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="E116" s="2"/>
-      <c r="F116" s="2"/>
-      <c r="G116" s="2">
-        <v>0</v>
-      </c>
-      <c r="H116" s="3">
+      <c r="G116">
+        <v>0</v>
+      </c>
+      <c r="H116" s="1">
         <v>44881.722314814811</v>
       </c>
-      <c r="I116" s="2" t="s">
+      <c r="I116" t="s">
         <v>113</v>
       </c>
-      <c r="J116" s="2">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A117" s="2" t="s">
+      <c r="J116">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>98</v>
       </c>
-      <c r="B117" s="2">
+      <c r="B117">
         <v>46</v>
       </c>
-      <c r="C117" s="2">
+      <c r="C117">
         <v>6.3E-2</v>
       </c>
-      <c r="D117" s="2">
+      <c r="D117">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="E117" s="2"/>
-      <c r="F117" s="2"/>
-      <c r="G117" s="2">
+      <c r="G117">
         <v>36.43</v>
       </c>
-      <c r="H117" s="3">
+      <c r="H117" s="1">
         <v>44881.72252314815</v>
       </c>
-      <c r="I117" s="2" t="s">
+      <c r="I117" t="s">
         <v>113</v>
       </c>
-      <c r="J117" s="2">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J117">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>99</v>
       </c>
@@ -3767,7 +3735,7 @@
         <v>44881.72314814815</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>100</v>
       </c>
@@ -3787,7 +3755,7 @@
         <v>44881.723356481481</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>101</v>
       </c>
@@ -3807,7 +3775,7 @@
         <v>44881.723981481482</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>102</v>
       </c>
@@ -3827,7 +3795,7 @@
         <v>44881.724189814813</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>4</v>
       </c>
@@ -3850,7 +3818,7 @@
         <v>44881.724814814814</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>8</v>
       </c>
@@ -3876,7 +3844,7 @@
         <v>44881.725023148145</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>11</v>
       </c>

</xml_diff>